<commit_message>
Onboard Skylar and Laura Soler with cleaned data
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/laurasoler/Laura_Soler_Complete_Infloww.xlsx
+++ b/laurasoler/Laura_Soler_Complete_Infloww.xlsx
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B32" s="8" t="inlineStr">
         <is>
-          <t>nice, I'm from Malaga but honestly I just go to the gym most of the time haha</t>
+          <t>nice, I'm from Spain but honestly I just go to the gym and run most of the time haha, when I'm not studying</t>
         </is>
       </c>
       <c r="C32" s="8" t="inlineStr"/>
@@ -3562,7 +3562,7 @@
       </c>
       <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>I'm 18, still figuring life out haha</t>
+          <t>I'm 18, just started this whole journey and honestly I love it</t>
         </is>
       </c>
       <c r="C2" s="9" t="inlineStr"/>
@@ -3585,12 +3585,12 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>I'm in Malaga but I don't really like sharing too many details about where exactly</t>
+          <t>I'm in Spain but I don't really like sharing too many details about where exactly</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>NEVER give specific neighborhood or address.</t>
+          <t>NEVER give specific city.</t>
         </is>
       </c>
     </row>
@@ -3602,7 +3602,7 @@
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>I do content creation full time, before this I was doing studying (prev: na)</t>
+          <t>I'm a student and I do content creation on the side, it kind of blew up honestly</t>
         </is>
       </c>
       <c r="C4" s="9" t="inlineStr"/>
@@ -3615,7 +3615,7 @@
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>I'm really into Gym, running, food: Vegetables, that's pretty much my life outside of this</t>
+          <t>I'm really into the gym and running, and I try to eat healthy but I'm not perfect haha</t>
         </is>
       </c>
       <c r="C5" s="9" t="inlineStr"/>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>I haven't traveled much yet but it's on my list for sure</t>
+          <t>I've been to Spain, the US, and Argentina, my parents are from there</t>
         </is>
       </c>
       <c r="C6" s="9" t="inlineStr"/>

</xml_diff>